<commit_message>
small fixes in task 1
</commit_message>
<xml_diff>
--- a/Lab2/Task-1/Data.xlsx
+++ b/Lab2/Task-1/Data.xlsx
@@ -369,49 +369,49 @@
         <v>0</v>
       </c>
       <c r="B1" t="n">
-        <v>-2.342114944842237</v>
+        <v>57.14571807951455</v>
       </c>
       <c r="C1" t="n">
-        <v>18.08771924798976</v>
+        <v>65.45588390529966</v>
       </c>
       <c r="D1" t="n">
-        <v>2.693617311165912</v>
+        <v>84.98174670937232</v>
       </c>
       <c r="E1" t="n">
-        <v>19.64044662508037</v>
+        <v>-35.50340589055043</v>
       </c>
       <c r="F1" t="n">
-        <v>-16.5343365372496</v>
+        <v>57.85298202279029</v>
       </c>
       <c r="G1" t="n">
-        <v>6.537830894826335</v>
+        <v>9.290402801141639</v>
       </c>
       <c r="H1" t="n">
-        <v>16.41028111947814</v>
+        <v>-50.55973039993673</v>
       </c>
       <c r="I1" t="n">
-        <v>-11.00057972107161</v>
+        <v>-68.13806777921256</v>
       </c>
       <c r="J1" t="n">
-        <v>-3.082014267900163</v>
+        <v>-22.32442281339111</v>
       </c>
       <c r="K1" t="n">
-        <v>-14.99582721364639</v>
+        <v>-26.38550494778482</v>
       </c>
       <c r="L1" t="n">
-        <v>3.393579198523653</v>
+        <v>-30.35129918917852</v>
       </c>
       <c r="M1" t="n">
-        <v>-17.82856180227399</v>
+        <v>44.79659810853599</v>
       </c>
       <c r="N1" t="n">
-        <v>3.470280303884877</v>
+        <v>53.10157927067019</v>
       </c>
       <c r="O1" t="n">
-        <v>2.554941199952005</v>
+        <v>86.58216866330858</v>
       </c>
       <c r="P1" t="n">
-        <v>-14.15431451412088</v>
+        <v>-17.10896178306069</v>
       </c>
     </row>
     <row r="2" spans="1:16">
@@ -419,49 +419,49 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>9.537163502402414</v>
+        <v>-6.186719900796248</v>
       </c>
       <c r="C2" t="n">
-        <v>19.00580861199557</v>
+        <v>8.933753480231374</v>
       </c>
       <c r="D2" t="n">
-        <v>-1.108742286593731</v>
+        <v>89.90615483809918</v>
       </c>
       <c r="E2" t="n">
-        <v>6.077333073867184</v>
+        <v>76.47735309733278</v>
       </c>
       <c r="F2" t="n">
-        <v>0.06003640063977045</v>
+        <v>89.40251760147339</v>
       </c>
       <c r="G2" t="n">
-        <v>2.670046107522182</v>
+        <v>-37.36677148442045</v>
       </c>
       <c r="H2" t="n">
-        <v>-15.35123585940571</v>
+        <v>19.02214525930287</v>
       </c>
       <c r="I2" t="n">
-        <v>-1.798705440968892</v>
+        <v>12.50723293051084</v>
       </c>
       <c r="J2" t="n">
-        <v>-4.625485060098363</v>
+        <v>-36.25046865710955</v>
       </c>
       <c r="K2" t="n">
-        <v>8.319241380865737</v>
+        <v>-4.71823884534659</v>
       </c>
       <c r="L2" t="n">
-        <v>-1.51924449138939</v>
+        <v>7.343408082669683</v>
       </c>
       <c r="M2" t="n">
-        <v>-2.56446997005872</v>
+        <v>93.07749420195671</v>
       </c>
       <c r="N2" t="n">
-        <v>14.22058041416471</v>
+        <v>-70.14850984229169</v>
       </c>
       <c r="O2" t="n">
-        <v>13.5977722607275</v>
+        <v>-18.77170567501881</v>
       </c>
       <c r="P2" t="n">
-        <v>-12.24851591338686</v>
+        <v>-37.06698665258534</v>
       </c>
     </row>
   </sheetData>

</xml_diff>